<commit_message>
Results of new GMM function
</commit_message>
<xml_diff>
--- a/COVSCA/Adjacency_matrix_men.xlsx
+++ b/COVSCA/Adjacency_matrix_men.xlsx
@@ -639,7 +639,7 @@
         <v>0</v>
       </c>
       <c r="M4" t="n">
-        <v>0</v>
+        <v>-0.208543246337598</v>
       </c>
       <c r="N4" t="n">
         <v>0</v>
@@ -660,7 +660,7 @@
         <v>0</v>
       </c>
       <c r="T4" t="n">
-        <v>0</v>
+        <v>0.166647238906365</v>
       </c>
       <c r="U4" t="n">
         <v>0.622176377549086</v>
@@ -701,7 +701,7 @@
         <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>0</v>
+        <v>0.234363995960803</v>
       </c>
       <c r="M5" t="n">
         <v>0</v>
@@ -763,7 +763,7 @@
         <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>-0.181734497257527</v>
       </c>
       <c r="L6" t="n">
         <v>0</v>
@@ -1135,7 +1135,7 @@
         <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>-0.181734497257527</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
@@ -1197,7 +1197,7 @@
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>0.234363995960804</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -1259,7 +1259,7 @@
         <v>0</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>-0.208543246337598</v>
       </c>
       <c r="D14" t="n">
         <v>0</v>
@@ -1714,7 +1714,7 @@
         <v>0</v>
       </c>
       <c r="C21" t="n">
-        <v>0</v>
+        <v>0.166647238906365</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>

</xml_diff>